<commit_message>
Added and made tabs for 5 new test cases for requirements being added to the MVP for ISR.
</commit_message>
<xml_diff>
--- a/documentation/ATP/source/procedures.xlsx
+++ b/documentation/ATP/source/procedures.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2337DD-770F-49D6-85A0-F303C1612B84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E2696A-205D-4B27-8E44-E08E8D75314E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="2880" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -17,8 +17,13 @@
     <sheet name="SSR4.3.1.3" sheetId="7" r:id="rId7"/>
     <sheet name="SSR4.3.1.4" sheetId="8" r:id="rId8"/>
     <sheet name="SSR4.3.1.5" sheetId="9" r:id="rId9"/>
-    <sheet name="SR4.6.3" sheetId="10" r:id="rId10"/>
-    <sheet name="SR4.6.4" sheetId="11" r:id="rId11"/>
+    <sheet name="SSR4.3.1.6" sheetId="12" r:id="rId10"/>
+    <sheet name="SAR4.3.1.6.1" sheetId="13" r:id="rId11"/>
+    <sheet name="SAR4.3.1.6.2" sheetId="14" r:id="rId12"/>
+    <sheet name="SSR4.3.1.7" sheetId="15" r:id="rId13"/>
+    <sheet name="SR4.4.1" sheetId="16" r:id="rId14"/>
+    <sheet name="SR4.6.3" sheetId="10" r:id="rId15"/>
+    <sheet name="SR4.6.4" sheetId="11" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="214">
   <si>
     <t>Title</t>
   </si>
@@ -682,6 +687,12 @@
   </si>
   <si>
     <t>Click on any component of the **Target GUI**</t>
+  </si>
+  <si>
+    <t>API Model Creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify SSR 4.3.1.6 - The Facile GUI shall contain a view that allows the user to build a graphical model of the generated API. </t>
   </si>
 </sst>
 </file>
@@ -1034,6 +1045,135 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1048,135 +1188,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,836 +1475,854 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.20703125" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="15.89453125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A10" s="28" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="31" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="19">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="62">
         <v>1</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="20"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="37" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-    </row>
-    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="37" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="63"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="37" t="s">
+      <c r="D23" s="61"/>
+      <c r="E23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="37" t="s">
+      <c r="D24" s="61"/>
+      <c r="E24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="37" t="s">
+      <c r="D25" s="61"/>
+      <c r="E25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-    </row>
-    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="37" t="s">
+      <c r="D26" s="61"/>
+      <c r="E26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
-    </row>
-    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="37" t="s">
+      <c r="D27" s="61"/>
+      <c r="E27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
-    </row>
-    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="63"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="37" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="21"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="64"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="41" t="s">
+      <c r="D29" s="61"/>
+      <c r="E29" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-    </row>
-    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A30" s="44">
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="47"/>
+    </row>
+    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
         <v>2</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="45"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="45"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="30"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="45"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="30"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="45"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="30"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="45"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="33"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="45"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="33"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="45"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="45"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="30"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="45"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="30"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
-    </row>
-    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="45"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="53"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="45"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="30"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="58"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="46"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="61"/>
-    </row>
-    <row r="43" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A43" s="44">
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="29">
         <v>3</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="49"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="45"/>
-      <c r="B44" s="55" t="s">
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="30"/>
+      <c r="B44" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="45"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="45"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="53"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="45"/>
-      <c r="B47" s="55" t="s">
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="30"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="30"/>
+      <c r="B47" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="45"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="45"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="53"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="45"/>
-      <c r="B50" s="55" t="s">
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="30"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
+      <c r="B50" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="45"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="33"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="46"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="53"/>
-    </row>
-    <row r="53" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A53" s="44">
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="30"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="28"/>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A53" s="29">
         <v>4</v>
       </c>
-      <c r="B53" s="47" t="s">
+      <c r="B53" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="49"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45" t="s">
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="33"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="33"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="33"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="33"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="33"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="33"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="33"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="53"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="25"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="25"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="25"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="25"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2307,32 +2336,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2340,6 +2351,1134 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="253.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="318.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2635D6-FB9F-46D2-BC35-410924B7C235}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B5E574-C0A0-410C-BD01-0D5765B42B4A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -2347,21 +3486,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5234375" customWidth="1"/>
-    <col min="2" max="2" width="55.3125" customWidth="1"/>
-    <col min="3" max="3" width="25.89453125" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="32.41796875" customWidth="1"/>
-    <col min="7" max="7" width="24.3125" customWidth="1"/>
-    <col min="8" max="8" width="25.1015625" customWidth="1"/>
-    <col min="9" max="9" width="18.89453125" customWidth="1"/>
-    <col min="10" max="10" width="21.68359375" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +3532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -2425,7 +3564,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2447,7 +3586,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2467,7 +3606,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2483,7 +3622,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2499,7 +3638,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2515,7 +3654,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2531,7 +3670,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2547,7 +3686,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2563,7 +3702,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2579,7 +3718,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2591,7 +3730,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2603,13 +3742,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
       <c r="J15" s="8"/>
     </row>
@@ -2618,7 +3757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85CACF-4790-4931-9075-36197B0BDD71}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -2626,20 +3765,20 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.68359375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="29.89453125" customWidth="1"/>
-    <col min="4" max="4" width="24.68359375" customWidth="1"/>
-    <col min="5" max="5" width="28.3125" customWidth="1"/>
-    <col min="6" max="6" width="26.89453125" customWidth="1"/>
-    <col min="7" max="7" width="24.1015625" customWidth="1"/>
-    <col min="8" max="8" width="21.1015625" customWidth="1"/>
-    <col min="9" max="10" width="26.1015625" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="9" max="10" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +3810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="225.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -2703,7 +3842,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2725,7 +3864,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2741,7 +3880,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2757,7 +3896,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2773,7 +3912,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2789,7 +3928,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2805,7 +3944,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2821,7 +3960,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2837,7 +3976,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2853,7 +3992,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2869,7 +4008,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2881,7 +4020,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -2898,22 +4037,22 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5234375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.20703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.20703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.1015625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="40" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.20703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="46.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="29" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.3125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="2"/>
+    <col min="10" max="10" width="29.33203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +4084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2977,7 +4116,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2999,7 +4138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3015,7 +4154,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3031,7 +4170,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3047,7 +4186,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3063,7 +4202,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3079,27 +4218,27 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14" s="8"/>
     </row>
   </sheetData>
@@ -3116,21 +4255,21 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3125" customWidth="1"/>
-    <col min="2" max="2" width="68.7890625" customWidth="1"/>
-    <col min="3" max="3" width="16.1015625" customWidth="1"/>
-    <col min="4" max="4" width="19.20703125" customWidth="1"/>
-    <col min="5" max="5" width="38.3125" customWidth="1"/>
-    <col min="6" max="6" width="17.7890625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="19.5234375" customWidth="1"/>
-    <col min="9" max="9" width="18.7890625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +4301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -3194,7 +4333,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3216,7 +4355,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3232,7 +4371,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3248,7 +4387,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3264,7 +4403,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3280,7 +4419,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3296,7 +4435,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3312,7 +4451,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3328,7 +4467,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3344,7 +4483,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3356,7 +4495,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3377,25 +4516,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B71E50-493D-4640-A992-202C8A3B64C0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.20703125" customWidth="1"/>
-    <col min="2" max="2" width="53.89453125" customWidth="1"/>
-    <col min="3" max="3" width="28.3125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.1015625" customWidth="1"/>
-    <col min="6" max="6" width="19.20703125" customWidth="1"/>
-    <col min="7" max="7" width="34.20703125" customWidth="1"/>
-    <col min="8" max="8" width="45.1015625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="22.3125" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +4566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -3459,7 +4598,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3481,7 +4620,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3501,7 +4640,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3517,7 +4656,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3533,7 +4672,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3549,7 +4688,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3565,7 +4704,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3581,7 +4720,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3597,7 +4736,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3613,7 +4752,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3629,7 +4768,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3641,7 +4780,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -3655,25 +4794,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E612745-E32A-4DF6-8B6E-CDF906DFB81F}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+    <sheetView topLeftCell="P3" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" customWidth="1"/>
-    <col min="2" max="2" width="52.7890625" customWidth="1"/>
-    <col min="3" max="3" width="18.3125" customWidth="1"/>
-    <col min="4" max="4" width="16.89453125" customWidth="1"/>
-    <col min="5" max="5" width="19.1015625" customWidth="1"/>
-    <col min="6" max="6" width="18.3125" customWidth="1"/>
-    <col min="7" max="7" width="28.41796875" customWidth="1"/>
-    <col min="8" max="8" width="39.41796875" customWidth="1"/>
-    <col min="9" max="9" width="29.5234375" customWidth="1"/>
-    <col min="10" max="10" width="26.20703125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3705,7 +4844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -3737,7 +4876,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3759,7 +4898,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3777,7 +4916,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3793,7 +4932,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3809,7 +4948,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3825,7 +4964,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3841,7 +4980,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3857,7 +4996,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3873,7 +5012,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3889,7 +5028,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3905,7 +5044,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3921,7 +5060,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -3938,21 +5077,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1015625" customWidth="1"/>
-    <col min="2" max="2" width="67.3125" customWidth="1"/>
-    <col min="3" max="3" width="39.7890625" customWidth="1"/>
-    <col min="4" max="4" width="39.89453125" customWidth="1"/>
-    <col min="5" max="5" width="32.41796875" customWidth="1"/>
-    <col min="6" max="6" width="26.1015625" customWidth="1"/>
-    <col min="7" max="7" width="28.20703125" customWidth="1"/>
-    <col min="8" max="8" width="30.1015625" customWidth="1"/>
-    <col min="9" max="9" width="24.68359375" customWidth="1"/>
-    <col min="10" max="10" width="23.7890625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3984,7 +5123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -4016,7 +5155,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4038,7 +5177,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4056,7 +5195,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4072,7 +5211,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4088,7 +5227,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4104,7 +5243,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4120,7 +5259,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4136,7 +5275,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4152,7 +5291,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4168,7 +5307,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4184,7 +5323,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4200,7 +5339,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>105</v>
       </c>
@@ -4208,7 +5347,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>106</v>
       </c>
@@ -4216,7 +5355,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>107</v>
       </c>
@@ -4224,7 +5363,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>108</v>
       </c>
@@ -4232,7 +5371,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
         <v>109</v>
       </c>
@@ -4253,21 +5392,21 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.68359375" customWidth="1"/>
-    <col min="2" max="2" width="49.20703125" customWidth="1"/>
-    <col min="3" max="3" width="31.20703125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="22.68359375" customWidth="1"/>
-    <col min="6" max="6" width="23.7890625" customWidth="1"/>
-    <col min="7" max="7" width="19.7890625" customWidth="1"/>
-    <col min="8" max="8" width="23.41796875" customWidth="1"/>
-    <col min="9" max="9" width="28.20703125" customWidth="1"/>
-    <col min="10" max="10" width="32.5234375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.21875" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" customWidth="1"/>
+    <col min="10" max="10" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4299,7 +5438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="141" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
@@ -4331,7 +5470,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4353,7 +5492,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4369,7 +5508,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4385,7 +5524,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4401,7 +5540,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4417,7 +5556,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4433,7 +5572,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4449,7 +5588,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4465,7 +5604,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4481,7 +5620,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4497,7 +5636,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4513,7 +5652,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -4530,21 +5669,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.68359375" customWidth="1"/>
-    <col min="2" max="2" width="63.5234375" customWidth="1"/>
-    <col min="3" max="3" width="33.3125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="37.1015625" customWidth="1"/>
-    <col min="6" max="6" width="30.1015625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="28.7890625" customWidth="1"/>
-    <col min="9" max="9" width="24.20703125" customWidth="1"/>
-    <col min="10" max="10" width="25.89453125" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4576,7 +5715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
@@ -4608,7 +5747,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4626,7 +5765,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4644,7 +5783,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4660,7 +5799,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4676,7 +5815,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4692,7 +5831,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4708,7 +5847,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4724,7 +5863,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4740,7 +5879,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4756,7 +5895,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4772,7 +5911,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4788,7 +5927,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>133</v>
       </c>
@@ -4796,7 +5935,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>137</v>
       </c>
@@ -4804,15 +5943,15 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G16" s="2"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="2"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="2"/>
       <c r="H18" s="16"/>
     </row>
@@ -4825,25 +5964,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7A820-7995-470D-BE20-79FB7431179A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.89453125" customWidth="1"/>
-    <col min="2" max="2" width="50.68359375" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="24.7890625" customWidth="1"/>
-    <col min="5" max="5" width="23.5234375" customWidth="1"/>
-    <col min="6" max="6" width="24.5234375" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="24.3125" customWidth="1"/>
-    <col min="9" max="9" width="22.41796875" customWidth="1"/>
-    <col min="10" max="10" width="23.41796875" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4875,7 +6014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>138</v>
       </c>
@@ -4907,7 +6046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4925,7 +6064,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4943,7 +6082,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4959,7 +6098,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4975,7 +6114,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4991,7 +6130,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5007,7 +6146,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5023,7 +6162,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5039,7 +6178,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5055,7 +6194,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5071,7 +6210,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5087,7 +6226,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>146</v>
       </c>
@@ -5095,7 +6234,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>

</xml_diff>

<commit_message>
5 new tabs for 5 requirements under MVP for ISR
</commit_message>
<xml_diff>
--- a/documentation/ATP/source/procedures.xlsx
+++ b/documentation/ATP/source/procedures.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2337DD-770F-49D6-85A0-F303C1612B84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E2696A-205D-4B27-8E44-E08E8D75314E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="2880" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -17,8 +17,13 @@
     <sheet name="SSR4.3.1.3" sheetId="7" r:id="rId7"/>
     <sheet name="SSR4.3.1.4" sheetId="8" r:id="rId8"/>
     <sheet name="SSR4.3.1.5" sheetId="9" r:id="rId9"/>
-    <sheet name="SR4.6.3" sheetId="10" r:id="rId10"/>
-    <sheet name="SR4.6.4" sheetId="11" r:id="rId11"/>
+    <sheet name="SSR4.3.1.6" sheetId="12" r:id="rId10"/>
+    <sheet name="SAR4.3.1.6.1" sheetId="13" r:id="rId11"/>
+    <sheet name="SAR4.3.1.6.2" sheetId="14" r:id="rId12"/>
+    <sheet name="SSR4.3.1.7" sheetId="15" r:id="rId13"/>
+    <sheet name="SR4.4.1" sheetId="16" r:id="rId14"/>
+    <sheet name="SR4.6.3" sheetId="10" r:id="rId15"/>
+    <sheet name="SR4.6.4" sheetId="11" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="214">
   <si>
     <t>Title</t>
   </si>
@@ -682,6 +687,12 @@
   </si>
   <si>
     <t>Click on any component of the **Target GUI**</t>
+  </si>
+  <si>
+    <t>API Model Creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify SSR 4.3.1.6 - The Facile GUI shall contain a view that allows the user to build a graphical model of the generated API. </t>
   </si>
 </sst>
 </file>
@@ -1034,6 +1045,135 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1048,135 +1188,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,836 +1475,854 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.20703125" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="15.89453125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A10" s="28" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="31" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="19">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="62">
         <v>1</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="20"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="37" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
-    </row>
-    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="37" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="63"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="37" t="s">
+      <c r="D23" s="61"/>
+      <c r="E23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="37" t="s">
+      <c r="D24" s="61"/>
+      <c r="E24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="37" t="s">
+      <c r="D25" s="61"/>
+      <c r="E25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-    </row>
-    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="37" t="s">
+      <c r="D26" s="61"/>
+      <c r="E26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
-    </row>
-    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="37" t="s">
+      <c r="D27" s="61"/>
+      <c r="E27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
-    </row>
-    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="63"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="37" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="21"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="64"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="41" t="s">
+      <c r="D29" s="61"/>
+      <c r="E29" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-    </row>
-    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A30" s="44">
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="47"/>
+    </row>
+    <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
         <v>2</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="45"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="45"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="30"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="45"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="30"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="45"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="30"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="45"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="33"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="45"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="33"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="45"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="45"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="30"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="45"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="30"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
-    </row>
-    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="45"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="53"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="45"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="30"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="58"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="46"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="61"/>
-    </row>
-    <row r="43" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A43" s="44">
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="29">
         <v>3</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="49"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="45"/>
-      <c r="B44" s="55" t="s">
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="30"/>
+      <c r="B44" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="45"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="45"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="53"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="45"/>
-      <c r="B47" s="55" t="s">
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="30"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="30"/>
+      <c r="B47" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="45"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="45"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="53"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="45"/>
-      <c r="B50" s="55" t="s">
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="30"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
+      <c r="B50" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="45"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="33"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="46"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="53"/>
-    </row>
-    <row r="53" spans="1:9" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A53" s="44">
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="30"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="28"/>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A53" s="29">
         <v>4</v>
       </c>
-      <c r="B53" s="47" t="s">
+      <c r="B53" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="49"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45" t="s">
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="33"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="33"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="33"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="33"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="33"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="33"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="33"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="53"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="25"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="25"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="25"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="25"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2307,32 +2336,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2340,6 +2351,1134 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="253.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="318.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2635D6-FB9F-46D2-BC35-410924B7C235}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B5E574-C0A0-410C-BD01-0D5765B42B4A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -2347,21 +3486,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5234375" customWidth="1"/>
-    <col min="2" max="2" width="55.3125" customWidth="1"/>
-    <col min="3" max="3" width="25.89453125" customWidth="1"/>
-    <col min="4" max="4" width="26.7890625" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="32.41796875" customWidth="1"/>
-    <col min="7" max="7" width="24.3125" customWidth="1"/>
-    <col min="8" max="8" width="25.1015625" customWidth="1"/>
-    <col min="9" max="9" width="18.89453125" customWidth="1"/>
-    <col min="10" max="10" width="21.68359375" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +3532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -2425,7 +3564,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2447,7 +3586,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2467,7 +3606,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2483,7 +3622,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2499,7 +3638,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2515,7 +3654,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2531,7 +3670,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2547,7 +3686,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2563,7 +3702,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2579,7 +3718,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2591,7 +3730,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2603,13 +3742,13 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
       <c r="J15" s="8"/>
     </row>
@@ -2618,7 +3757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85CACF-4790-4931-9075-36197B0BDD71}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -2626,20 +3765,20 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.68359375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="29.89453125" customWidth="1"/>
-    <col min="4" max="4" width="24.68359375" customWidth="1"/>
-    <col min="5" max="5" width="28.3125" customWidth="1"/>
-    <col min="6" max="6" width="26.89453125" customWidth="1"/>
-    <col min="7" max="7" width="24.1015625" customWidth="1"/>
-    <col min="8" max="8" width="21.1015625" customWidth="1"/>
-    <col min="9" max="10" width="26.1015625" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="9" max="10" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +3810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="225.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -2703,7 +3842,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2725,7 +3864,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2741,7 +3880,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2757,7 +3896,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2773,7 +3912,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2789,7 +3928,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2805,7 +3944,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2821,7 +3960,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2837,7 +3976,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2853,7 +3992,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2869,7 +4008,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2881,7 +4020,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -2898,22 +4037,22 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5234375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.20703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.20703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.1015625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="40" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.20703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="46.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="29" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.3125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="2"/>
+    <col min="10" max="10" width="29.33203125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +4084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2977,7 +4116,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2999,7 +4138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3015,7 +4154,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3031,7 +4170,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3047,7 +4186,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3063,7 +4202,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3079,27 +4218,27 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14" s="8"/>
     </row>
   </sheetData>
@@ -3116,21 +4255,21 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3125" customWidth="1"/>
-    <col min="2" max="2" width="68.7890625" customWidth="1"/>
-    <col min="3" max="3" width="16.1015625" customWidth="1"/>
-    <col min="4" max="4" width="19.20703125" customWidth="1"/>
-    <col min="5" max="5" width="38.3125" customWidth="1"/>
-    <col min="6" max="6" width="17.7890625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="19.5234375" customWidth="1"/>
-    <col min="9" max="9" width="18.7890625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" customWidth="1"/>
     <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +4301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -3194,7 +4333,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3216,7 +4355,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3232,7 +4371,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3248,7 +4387,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3264,7 +4403,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3280,7 +4419,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3296,7 +4435,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3312,7 +4451,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3328,7 +4467,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3344,7 +4483,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3356,7 +4495,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3377,25 +4516,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B71E50-493D-4640-A992-202C8A3B64C0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.20703125" customWidth="1"/>
-    <col min="2" max="2" width="53.89453125" customWidth="1"/>
-    <col min="3" max="3" width="28.3125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.1015625" customWidth="1"/>
-    <col min="6" max="6" width="19.20703125" customWidth="1"/>
-    <col min="7" max="7" width="34.20703125" customWidth="1"/>
-    <col min="8" max="8" width="45.1015625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="22.3125" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +4566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -3459,7 +4598,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3481,7 +4620,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3501,7 +4640,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3517,7 +4656,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3533,7 +4672,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3549,7 +4688,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3565,7 +4704,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3581,7 +4720,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3597,7 +4736,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3613,7 +4752,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3629,7 +4768,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3641,7 +4780,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -3655,25 +4794,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E612745-E32A-4DF6-8B6E-CDF906DFB81F}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+    <sheetView topLeftCell="P3" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" customWidth="1"/>
-    <col min="2" max="2" width="52.7890625" customWidth="1"/>
-    <col min="3" max="3" width="18.3125" customWidth="1"/>
-    <col min="4" max="4" width="16.89453125" customWidth="1"/>
-    <col min="5" max="5" width="19.1015625" customWidth="1"/>
-    <col min="6" max="6" width="18.3125" customWidth="1"/>
-    <col min="7" max="7" width="28.41796875" customWidth="1"/>
-    <col min="8" max="8" width="39.41796875" customWidth="1"/>
-    <col min="9" max="9" width="29.5234375" customWidth="1"/>
-    <col min="10" max="10" width="26.20703125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3705,7 +4844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -3737,7 +4876,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3759,7 +4898,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3777,7 +4916,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3793,7 +4932,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3809,7 +4948,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3825,7 +4964,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3841,7 +4980,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3857,7 +4996,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3873,7 +5012,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3889,7 +5028,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3905,7 +5044,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3921,7 +5060,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -3938,21 +5077,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1015625" customWidth="1"/>
-    <col min="2" max="2" width="67.3125" customWidth="1"/>
-    <col min="3" max="3" width="39.7890625" customWidth="1"/>
-    <col min="4" max="4" width="39.89453125" customWidth="1"/>
-    <col min="5" max="5" width="32.41796875" customWidth="1"/>
-    <col min="6" max="6" width="26.1015625" customWidth="1"/>
-    <col min="7" max="7" width="28.20703125" customWidth="1"/>
-    <col min="8" max="8" width="30.1015625" customWidth="1"/>
-    <col min="9" max="9" width="24.68359375" customWidth="1"/>
-    <col min="10" max="10" width="23.7890625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3984,7 +5123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -4016,7 +5155,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4038,7 +5177,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4056,7 +5195,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4072,7 +5211,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4088,7 +5227,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4104,7 +5243,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4120,7 +5259,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4136,7 +5275,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4152,7 +5291,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4168,7 +5307,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4184,7 +5323,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4200,7 +5339,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>105</v>
       </c>
@@ -4208,7 +5347,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>106</v>
       </c>
@@ -4216,7 +5355,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>107</v>
       </c>
@@ -4224,7 +5363,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>108</v>
       </c>
@@ -4232,7 +5371,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
         <v>109</v>
       </c>
@@ -4253,21 +5392,21 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.68359375" customWidth="1"/>
-    <col min="2" max="2" width="49.20703125" customWidth="1"/>
-    <col min="3" max="3" width="31.20703125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="22.68359375" customWidth="1"/>
-    <col min="6" max="6" width="23.7890625" customWidth="1"/>
-    <col min="7" max="7" width="19.7890625" customWidth="1"/>
-    <col min="8" max="8" width="23.41796875" customWidth="1"/>
-    <col min="9" max="9" width="28.20703125" customWidth="1"/>
-    <col min="10" max="10" width="32.5234375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.21875" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" customWidth="1"/>
+    <col min="10" max="10" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4299,7 +5438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="141" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
@@ -4331,7 +5470,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4353,7 +5492,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4369,7 +5508,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4385,7 +5524,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4401,7 +5540,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4417,7 +5556,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4433,7 +5572,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4449,7 +5588,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4465,7 +5604,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4481,7 +5620,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4497,7 +5636,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4513,7 +5652,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -4530,21 +5669,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.68359375" customWidth="1"/>
-    <col min="2" max="2" width="63.5234375" customWidth="1"/>
-    <col min="3" max="3" width="33.3125" customWidth="1"/>
-    <col min="4" max="4" width="31.1015625" customWidth="1"/>
-    <col min="5" max="5" width="37.1015625" customWidth="1"/>
-    <col min="6" max="6" width="30.1015625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="28.7890625" customWidth="1"/>
-    <col min="9" max="9" width="24.20703125" customWidth="1"/>
-    <col min="10" max="10" width="25.89453125" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4576,7 +5715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="188.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
@@ -4608,7 +5747,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4626,7 +5765,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4644,7 +5783,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4660,7 +5799,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4676,7 +5815,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4692,7 +5831,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4708,7 +5847,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4724,7 +5863,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4740,7 +5879,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4756,7 +5895,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4772,7 +5911,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4788,7 +5927,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>133</v>
       </c>
@@ -4796,7 +5935,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>137</v>
       </c>
@@ -4804,15 +5943,15 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G16" s="2"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="2"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="2"/>
       <c r="H18" s="16"/>
     </row>
@@ -4825,25 +5964,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7A820-7995-470D-BE20-79FB7431179A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.89453125" customWidth="1"/>
-    <col min="2" max="2" width="50.68359375" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="24.7890625" customWidth="1"/>
-    <col min="5" max="5" width="23.5234375" customWidth="1"/>
-    <col min="6" max="6" width="24.5234375" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="24.3125" customWidth="1"/>
-    <col min="9" max="9" width="22.41796875" customWidth="1"/>
-    <col min="10" max="10" width="23.41796875" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.200000000000003" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4875,7 +6014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="221.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>138</v>
       </c>
@@ -4907,7 +6046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4925,7 +6064,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4943,7 +6082,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4959,7 +6098,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4975,7 +6114,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4991,7 +6130,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5007,7 +6146,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5023,7 +6162,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5039,7 +6178,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5055,7 +6194,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5071,7 +6210,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -5087,7 +6226,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>146</v>
       </c>
@@ -5095,7 +6234,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>

</xml_diff>

<commit_message>
Did some more work on test cases but not finished.
</commit_message>
<xml_diff>
--- a/documentation/ATP/source/procedures.xlsx
+++ b/documentation/ATP/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E2696A-205D-4B27-8E44-E08E8D75314E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFEA7CE-6327-498F-B6AE-146015CEA2B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="2880" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17460" yWindow="744" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,8 @@
     <sheet name="SAR4.3.1.6.1" sheetId="13" r:id="rId11"/>
     <sheet name="SAR4.3.1.6.2" sheetId="14" r:id="rId12"/>
     <sheet name="SSR4.3.1.7" sheetId="15" r:id="rId13"/>
-    <sheet name="SR4.4.1" sheetId="16" r:id="rId14"/>
-    <sheet name="SR4.6.3" sheetId="10" r:id="rId15"/>
-    <sheet name="SR4.6.4" sheetId="11" r:id="rId16"/>
+    <sheet name="SR4.6.3" sheetId="10" r:id="rId14"/>
+    <sheet name="SR4.6.4" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="225">
   <si>
     <t>Title</t>
   </si>
@@ -693,6 +692,39 @@
   </si>
   <si>
     <t xml:space="preserve">To verify SSR 4.3.1.6 - The Facile GUI shall contain a view that allows the user to build a graphical model of the generated API. </t>
+  </si>
+  <si>
+    <t>Action Pipeline Creation</t>
+  </si>
+  <si>
+    <t>To verify SAR 4.3.1.6.1 - The Facile GUI shall allow the user to create action pipelines utilizing predefined actions.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to build a model of the API model they generated.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to create action pipelines from predefined actions.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>Show Relevant Actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify SAR4.3.1.6.2 - The Facile GUI shall contain a view that shows all actions relevant to the target GUI model. </t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that shows any action that is relevant to the target GUI model.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>Validator</t>
+  </si>
+  <si>
+    <t>To verify SSR4.3.1.7 - The Facile GUI shall contain a view that warns the user of potential errors in project models.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view with a  dialog that will let the user know of any potential errors for the project model being used.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>Context menu of items will be shown.</t>
   </si>
 </sst>
 </file>
@@ -1045,6 +1077,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,21 +1179,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1082,13 +1189,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,15 +1197,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1125,69 +1220,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,846 +1515,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="53"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="62">
+      <c r="A19" s="19">
         <v>1</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="59"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="63"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="21" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="21" t="s">
+      <c r="D23" s="18"/>
+      <c r="E23" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="21" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="22"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="22"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="21" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="22"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="63"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="36" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="29">
+      <c r="A30" s="44">
         <v>2</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="49"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="22"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="25"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="33"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="33"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
+      <c r="A36" s="45"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="25"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="33"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="30"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="43"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="64"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
+      <c r="A38" s="45"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="22"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="30"/>
+      <c r="A39" s="45"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="25"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="30"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="28"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="53"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="58"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="61"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="29">
+      <c r="A43" s="44">
         <v>3</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="19"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="49"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
-      <c r="B44" s="32" t="s">
+      <c r="A44" s="45"/>
+      <c r="B44" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="22"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="38"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="25"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="33"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="28"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="53"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
-      <c r="B47" s="32" t="s">
+      <c r="A47" s="45"/>
+      <c r="B47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="25"/>
+      <c r="A48" s="45"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="33"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="30"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="28"/>
+      <c r="A49" s="45"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="53"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
-      <c r="B50" s="32" t="s">
+      <c r="A50" s="45"/>
+      <c r="B50" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="22"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="38"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="25"/>
+      <c r="A51" s="45"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="33"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="31"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="28"/>
+      <c r="A52" s="46"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="53"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="29">
+      <c r="A53" s="44">
         <v>4</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="19"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="49"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30" t="s">
+      <c r="A54" s="45"/>
+      <c r="B54" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="22"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="38"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="25"/>
+      <c r="A55" s="45"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="33"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="25"/>
+      <c r="A56" s="45"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="33"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="25"/>
+      <c r="A57" s="45"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="33"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="25"/>
+      <c r="A58" s="45"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="33"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="25"/>
+      <c r="A59" s="45"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="33"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="25"/>
+      <c r="A60" s="45"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="33"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="25"/>
+      <c r="A61" s="45"/>
+      <c r="B61" s="45"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="33"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="25"/>
+      <c r="A62" s="45"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="33"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="28"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2336,14 +2350,32 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2354,8 +2386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2372,7 +2404,7 @@
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2409,7 +2441,7 @@
         <v>212</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2429,12 +2461,8 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>150</v>
-      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -2454,7 +2482,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2472,7 +2500,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2488,7 +2516,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2504,7 +2532,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2520,7 +2548,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2536,7 +2564,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2552,77 +2580,57 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>148</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2633,13 +2641,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
@@ -2651,7 +2659,7 @@
     <col min="10" max="10" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2685,10 +2693,10 @@
     </row>
     <row r="2" spans="1:10" ht="253.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2697,7 +2705,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>139</v>
+        <v>215</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -2708,14 +2716,10 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2733,7 +2737,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2751,7 +2755,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2767,7 +2771,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2783,7 +2787,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2799,7 +2803,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2815,7 +2819,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2831,77 +2835,57 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>148</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2912,14 +2896,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:J14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
@@ -2930,7 +2914,7 @@
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2962,12 +2946,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2976,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -2987,12 +2971,8 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>150</v>
-      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -3012,7 +2992,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3030,7 +3010,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3046,7 +3026,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3062,7 +3042,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3078,7 +3058,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3094,7 +3074,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3110,77 +3090,57 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>148</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3191,14 +3151,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
@@ -3209,7 +3169,7 @@
     <col min="10" max="10" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3241,12 +3201,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="318.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="295.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>221</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3255,7 +3215,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>139</v>
+        <v>222</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -3266,12 +3226,8 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>150</v>
-      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -3291,7 +3247,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3309,7 +3265,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3325,7 +3281,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3341,7 +3297,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3357,7 +3313,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3373,7 +3329,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3389,7 +3345,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3400,66 +3356,50 @@
         <v>140</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>115</v>
+        <v>224</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>148</v>
-      </c>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3467,18 +3407,6 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2635D6-FB9F-46D2-BC35-410924B7C235}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B5E574-C0A0-410C-BD01-0D5765B42B4A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -3757,7 +3685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85CACF-4790-4931-9075-36197B0BDD71}">
   <dimension ref="A1:J14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed new test cases. Trying to fix bugs from laTex.
</commit_message>
<xml_diff>
--- a/documentation/ATP/source/procedures.xlsx
+++ b/documentation/ATP/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFEA7CE-6327-498F-B6AE-146015CEA2B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEF7208-8A95-4A08-B455-C29ED8022768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17460" yWindow="744" windowWidth="17280" windowHeight="11508" tabRatio="683" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="288">
   <si>
     <t>Title</t>
   </si>
@@ -700,31 +700,220 @@
     <t>To verify SAR 4.3.1.6.1 - The Facile GUI shall allow the user to create action pipelines utilizing predefined actions.</t>
   </si>
   <si>
-    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to build a model of the API model they generated.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
-  </si>
-  <si>
-    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to create action pipelines from predefined actions.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
-  </si>
-  <si>
     <t>Show Relevant Actions</t>
   </si>
   <si>
     <t xml:space="preserve">To verify SAR4.3.1.6.2 - The Facile GUI shall contain a view that shows all actions relevant to the target GUI model. </t>
   </si>
   <si>
-    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that shows any action that is relevant to the target GUI model.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
-  </si>
-  <si>
     <t>Validator</t>
   </si>
   <si>
     <t>To verify SSR4.3.1.7 - The Facile GUI shall contain a view that warns the user of potential errors in project models.</t>
   </si>
   <si>
-    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view with a  dialog that will let the user know of any potential errors for the project model being used.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
-  </si>
-  <si>
-    <t>Context menu of items will be shown.</t>
+    <t>Click on a component in the **Create New Action Pipeline**</t>
+  </si>
+  <si>
+    <t>Dialog box to add **Input Ports** and **Output Ports** is shown in a new window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on **default** under **Input Ports** and add a name. </t>
+  </si>
+  <si>
+    <t>Name of input port is updated.</t>
+  </si>
+  <si>
+    <t>Click on **NoneType** under **Input Ports** and add the type data structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of data structure for input port is updated. </t>
+  </si>
+  <si>
+    <t>Decide whether to make the value of the input port required or optional.</t>
+  </si>
+  <si>
+    <t>Value of input port is updated or not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on **Edit ports for:** and add a name. </t>
+  </si>
+  <si>
+    <t>Name of ports for action pipeline is updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on **default** under **Output Ports** and add a name. </t>
+  </si>
+  <si>
+    <t>Name of output port is updated.</t>
+  </si>
+  <si>
+    <t>Click on **NoneType** under **Output Ports** and add the type data structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of data structure for output port is updated. </t>
+  </si>
+  <si>
+    <t>Click on **OK**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on **Validate TGUIM and API** icon. </t>
+  </si>
+  <si>
+    <t>Validator_test_01.png</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile software system that shows 200 messages of the TGUIM and API being validated for errors, warning, and info.</t>
+  </si>
+  <si>
+    <t>A variety of files are shown. The main file is the name of your project with the *.fcl* extension. Refer to @extension_test_01.png Test case is completed.</t>
+  </si>
+  <si>
+    <t>Value of input port is updated.</t>
+  </si>
+  <si>
+    <t>Click on **NoneType** under **Output Ports** and add the type of data structure.</t>
+  </si>
+  <si>
+    <t>ShowRelevantActions_test_01.png</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile software system that shows all relevant actions of the target GUI model in a Action Menu view under the Action Pipelines tab.</t>
+  </si>
+  <si>
+    <t>ActionPipelineCreation_test_01.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A snippit of the Facile system action pipeline creation dialog. This Black Box Editor allows the user to add input and/or output ports to create an action pipeline. </t>
+  </si>
+  <si>
+    <t>ActionPipelineCreation_test_02.png</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to build a model of the API they generated with multiple action pipelines. User will be able to manipulate these action pipelines in the Action Menu by adding an action pipeline to a current action pipeline, editing the behavior or interface of the pipeline, and deleting the action pipeline.This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that will allow the user to create action pipelines from predefined actions. User will be able to add as many input or output ports of basic python data structures. This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view that shows any action that is relevant to the target GUI model. User will be able to choose from a Component Actions or Action Pipelines tab to modify the current action pipelines.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that contains a view with a  dialog that will let the user know of any potential errors for the project model being used.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing. User will be able to hide or show info, warning, or error messages in a Validator view. It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_01.png</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_02.png</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_03.png</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_04.png</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows an action pipeline in the API Model view with 4 input and output ports with the basic python data structures such as int, bool, float, and string.</t>
+  </si>
+  <si>
+    <t>Target GUI model is shown in the view.</t>
+  </si>
+  <si>
+    <t>Click on the **Create New Action Pipeline** icon.</t>
+  </si>
+  <si>
+    <t>Repeat past 5 steps till there is an input port and output port for bool, int, string, and float data types.</t>
+  </si>
+  <si>
+    <t>ActionPipelineCreation_test_03.png</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system action pipeline creation dialog that shows input and output ports of  bool, int, string, and float data types being added to the action pipeline.</t>
+  </si>
+  <si>
+    <t>Dialog box with 4 input ports and output ports with data types of bool, int, string, and float are added.</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_05.png</t>
+  </si>
+  <si>
+    <t>APIMCreation_test_06.png</t>
+  </si>
+  <si>
+    <t>Right click on an action in the **Action Menu** and click on **Add to Current Action Pipeline** to add an action pipeline to the current action pipeline.</t>
+  </si>
+  <si>
+    <t>Right click on an action in the **Action Menu** and click on **Add to Current Action Pipeline** to add another action pipeline to the current action pipeline.</t>
+  </si>
+  <si>
+    <t>Right click on an action in the API Model view and click on **delete** to delete an action pipeline from the current action pipeline.</t>
+  </si>
+  <si>
+    <t>Repeat the last step several times.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on a input port at the top level of an action pipeline and draw a wire from it to an top level output port or a child input port with the same data type. </t>
+  </si>
+  <si>
+    <t>A wire is drawn from an input port to a top level output port or a child input port with the same data type.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wave cursor over the an action pipeline. </t>
+  </si>
+  <si>
+    <t>Blue up and down arrow box is shown.</t>
+  </si>
+  <si>
+    <t>Click on blue up and down arrow to move an action pipeline up or down.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows an action pipeline being added to the current action pipeline in the API Model view.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows another action pipeline being added to the current action pipeline in the API Model view.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows an action pipeline with several input and output ports connected with wires. API Model view.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows an action pipeline with a modified alignment of the two action pipelines added to it with their wire port connections in the API Model view.</t>
+  </si>
+  <si>
+    <t>A snippit of the Facile system that shows an action pipeline that has been deleted from the current action pipeline in the API Model view.</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_03.png</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_04.png</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_05.png</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_06.png Test case is completed.</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_01.png</t>
+  </si>
+  <si>
+    <t>Refer to @APIMCreation_test_02.png</t>
+  </si>
+  <si>
+    <t>Refer to @ActionPipelineCreation_test_03.png Test Case is completed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to @ActionPipelineCreation_test_02.png </t>
+  </si>
+  <si>
+    <t>A action pipeline creation dialog is shown in a new window. Refer to @ActionPipelineCreation_test_01.png</t>
+  </si>
+  <si>
+    <t>Refer to @ShowRelevantActions_test_01.png Test Case is completed.</t>
+  </si>
+  <si>
+    <t>Refer to @Validator_test_01.png  Test case is completed</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1077,20 +1266,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1119,15 +1386,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1137,89 +1395,23 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,828 +1707,846 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="62">
         <v>1</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="37" t="s">
+      <c r="D20" s="61"/>
+      <c r="E20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="37" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="37" t="s">
+      <c r="D23" s="61"/>
+      <c r="E23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="63"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="37" t="s">
+      <c r="D24" s="61"/>
+      <c r="E24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="37" t="s">
+      <c r="D25" s="61"/>
+      <c r="E25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="37" t="s">
+      <c r="D26" s="61"/>
+      <c r="E26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="37" t="s">
+      <c r="D27" s="61"/>
+      <c r="E27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="37" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="41" t="s">
+      <c r="D29" s="61"/>
+      <c r="E29" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="47"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="44">
+      <c r="A30" s="29">
         <v>2</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="45"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="33"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="33"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="33"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="33"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="33"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="53"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="58"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="61"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="44">
+      <c r="A43" s="29">
         <v>3</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="49"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="45"/>
-      <c r="B44" s="55" t="s">
+      <c r="A44" s="30"/>
+      <c r="B44" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="45"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="33"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="53"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45"/>
-      <c r="B47" s="55" t="s">
+      <c r="A47" s="30"/>
+      <c r="B47" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="45"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="33"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="45"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="53"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="28"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="45"/>
-      <c r="B50" s="55" t="s">
+      <c r="A50" s="30"/>
+      <c r="B50" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="45"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="33"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="46"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="53"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="28"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="44">
+      <c r="A53" s="29">
         <v>4</v>
       </c>
-      <c r="B53" s="47" t="s">
+      <c r="B53" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="49"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45" t="s">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="33"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="25"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="33"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="33"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="25"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="33"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="33"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="33"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="25"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="25"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="33"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="25"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="53"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2350,32 +2560,14 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2384,10 +2576,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,10 +2590,10 @@
     <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
     <col min="9" max="9" width="19.21875" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2440,8 +2632,8 @@
       <c r="A2" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>216</v>
+      <c r="B2" s="65" t="s">
+        <v>246</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2449,7 +2641,7 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="65" t="s">
         <v>213</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -2461,10 +2653,14 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="I2" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2479,10 +2675,14 @@
       <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2497,10 +2697,14 @@
       <c r="H4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I4" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2513,10 +2717,14 @@
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="I5" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2529,10 +2737,14 @@
       <c r="H6" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2545,8 +2757,12 @@
       <c r="H7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -2580,83 +2796,216 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G24" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>280</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2691,12 +3040,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="253.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>217</v>
+      <c r="B2" s="65" t="s">
+        <v>247</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2704,7 +3053,7 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="65" t="s">
         <v>215</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -2716,10 +3065,14 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="I2" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2734,10 +3087,14 @@
       <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2752,10 +3109,14 @@
       <c r="H4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I4" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2771,7 +3132,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2787,7 +3148,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2819,7 +3180,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2835,57 +3196,127 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>283</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2894,10 +3325,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0C746B-3182-4B37-8AF4-A9D404711DCD}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2948,10 +3379,10 @@
     </row>
     <row r="2" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>248</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2959,8 +3390,8 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>219</v>
+      <c r="E2" s="65" t="s">
+        <v>217</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -2971,8 +3402,12 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -3090,57 +3525,117 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3151,8 +3646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3203,10 +3698,10 @@
     </row>
     <row r="2" spans="1:10" ht="295.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>249</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3214,8 +3709,8 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>222</v>
+      <c r="E2" s="65" t="s">
+        <v>219</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -3226,8 +3721,12 @@
       <c r="H2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -3345,7 +3844,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3353,35 +3852,43 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>224</v>
+        <v>118</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
     </row>
@@ -3410,8 +3917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B5E574-C0A0-410C-BD01-0D5765B42B4A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3630,7 +4137,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3641,7 +4148,7 @@
         <v>152</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -3689,7 +4196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85CACF-4790-4931-9075-36197B0BDD71}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -4444,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B71E50-493D-4640-A992-202C8A3B64C0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5593,8 +6100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83044C7C-9E56-4B9C-9D9C-01FE54DD804F}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5892,7 +6399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7A820-7995-470D-BE20-79FB7431179A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made some changes to the images and procedures.
</commit_message>
<xml_diff>
--- a/documentation/ATP/source/procedures.xlsx
+++ b/documentation/ATP/source/procedures.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEF7208-8A95-4A08-B455-C29ED8022768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00471FB9-A092-41B8-A331-E9EC6EDFE1C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -24,17 +24,25 @@
     <sheet name="SR4.6.3" sheetId="10" r:id="rId14"/>
     <sheet name="SR4.6.4" sheetId="11" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="289">
   <si>
     <t>Title</t>
   </si>
@@ -542,11 +550,6 @@
     <t>This acceptance test verifies that the software system, Facile is functional while using a Python 3.7.4 interpreter.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required with the intended programming language. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
   </si>
   <si>
-    <t>This acceptance test verifies that the software system, Facile has a functional GUI that interacts with the user.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.
-.. note::
-    The requirement that this test case is verifying is not completed yet because sub-system and sub-assembly requirements must first be completed.</t>
-  </si>
-  <si>
     <t>This acceptance test verifies that the software system, Facile has a view that will allow the user to identify components of a target GUI.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the target GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
   </si>
   <si>
@@ -914,6 +917,12 @@
   </si>
   <si>
     <t>Refer to @Validator_test_01.png  Test case is completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project is saved with the *.fcl* extension in the selected folder. Refer to @GUI_test_02.png </t>
+  </si>
+  <si>
+    <t>This acceptance test verifies that the software system, Facile has a functional GUI that interacts with the user.  This acceptance test establishes the framework used by the acceptance test team to plan, execute, and document acceptance testing.  It describes the scope of the work performed and the approach taken to execute the tests created to validate that the system performs as required in the GUI. The details of this acceptance test are developed according to the requirements specifications and show traceability back to those specifications.</t>
   </si>
 </sst>
 </file>
@@ -1266,98 +1275,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1386,6 +1320,15 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1395,23 +1338,89 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1707,846 +1716,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="53"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="25"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="62">
+      <c r="A19" s="20">
         <v>1</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="59"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" spans="1:9" ht="20.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="63"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="21" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="19"/>
+      <c r="E22" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="21" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="21" t="s">
+      <c r="D24" s="19"/>
+      <c r="E24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="22"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="22"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="1:9" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="21" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="22"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="63"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="36" t="s">
+      <c r="D29" s="19"/>
+      <c r="E29" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="29">
+      <c r="A30" s="45">
         <v>2</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="22"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="25"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="25"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="30"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="43"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="65"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="11"/>
       <c r="C38" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="22"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="30"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="25"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="34"/>
     </row>
     <row r="40" spans="1:9" ht="18.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="30"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="28"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="11"/>
       <c r="C41" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="29">
+      <c r="A43" s="45">
         <v>3</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="19"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="50"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
-      <c r="B44" s="32" t="s">
+      <c r="A44" s="46"/>
+      <c r="B44" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="22"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="39"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="25"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="28"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="54"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
-      <c r="B47" s="32" t="s">
+      <c r="A47" s="46"/>
+      <c r="B47" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="25"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="34"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="30"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="28"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
-      <c r="B50" s="32" t="s">
+      <c r="A50" s="46"/>
+      <c r="B50" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="22"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="39"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="25"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="34"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="31"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="28"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="54"/>
     </row>
     <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="29">
+      <c r="A53" s="45">
         <v>4</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="19"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="50"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30" t="s">
+      <c r="A54" s="46"/>
+      <c r="B54" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="22"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="39"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="25"/>
+      <c r="A55" s="46"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="34"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="25"/>
+      <c r="A56" s="46"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="34"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="25"/>
+      <c r="A57" s="46"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="34"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="25"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="25"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="25"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="34"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="25"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="34"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="25"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="34"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="28"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="C54:I63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A43:A52"/>
     <mergeCell ref="A30:A42"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="D47:I49"/>
@@ -2560,14 +2551,32 @@
     <mergeCell ref="D44:I46"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C54:I63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B54:B63"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2578,7 +2587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DEC4C-0859-492A-9859-A5102CF1C24C}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+    <sheetView topLeftCell="D18" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -2630,10 +2639,10 @@
     </row>
     <row r="2" spans="1:10" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>246</v>
+        <v>211</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>245</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -2641,23 +2650,23 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="65" t="s">
-        <v>213</v>
+      <c r="E2" s="17" t="s">
+        <v>212</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2676,10 +2685,10 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2698,10 +2707,10 @@
         <v>84</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2718,10 +2727,10 @@
         <v>21</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -2732,16 +2741,16 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2758,10 +2767,10 @@
         <v>115</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2836,10 +2845,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -2852,10 +2861,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
@@ -2868,116 +2877,116 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H16" s="16" t="s">
         <v>226</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="19" spans="7:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G20" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G21" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G22" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="7:8" ht="144" x14ac:dyDescent="0.3">
       <c r="G23" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H23" s="16" t="s">
         <v>267</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="24" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G24" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="7:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="G25" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H25" s="16" t="s">
         <v>269</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="26" spans="7:8" ht="72" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="7:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="G27" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2990,7 +2999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D9C558-86BD-4789-80C1-D36E81752C81}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3042,10 +3051,10 @@
     </row>
     <row r="2" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>247</v>
+        <v>213</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>246</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3053,23 +3062,23 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="65" t="s">
-        <v>215</v>
+      <c r="E2" s="17" t="s">
+        <v>214</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3088,10 +3097,10 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3110,10 +3119,10 @@
         <v>84</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3140,10 +3149,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -3223,7 +3232,7 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -3236,10 +3245,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -3252,70 +3261,70 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H16" s="16" t="s">
         <v>226</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="18" spans="7:8" ht="72" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="19" spans="7:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="7:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="G20" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3379,10 +3388,10 @@
     </row>
     <row r="2" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>248</v>
+        <v>215</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>247</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3390,23 +3399,23 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="65" t="s">
-        <v>217</v>
+      <c r="E2" s="17" t="s">
+        <v>216</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -3469,10 +3478,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -3552,7 +3561,7 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -3565,10 +3574,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -3581,60 +3590,60 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="18" spans="7:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="7:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3646,7 +3655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D9410B-47BB-4E45-80F2-F71FCE9008EE}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -3698,10 +3707,10 @@
     </row>
     <row r="2" spans="1:10" ht="295.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>249</v>
+        <v>217</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>248</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3709,23 +3718,23 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="65" t="s">
-        <v>219</v>
+      <c r="E2" s="17" t="s">
+        <v>218</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -3788,10 +3797,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -3871,7 +3880,7 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -3884,10 +3893,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -3917,8 +3926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B5E574-C0A0-410C-BD01-0D5765B42B4A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3972,7 +3981,7 @@
         <v>151</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -3987,10 +3996,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>89</v>
@@ -4065,10 +4074,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -4148,7 +4157,7 @@
         <v>152</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4194,10 +4203,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85CACF-4790-4931-9075-36197B0BDD71}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4250,7 +4259,7 @@
         <v>156</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -4265,10 +4274,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>89</v>
@@ -4277,7 +4286,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4293,13 +4302,13 @@
         <v>83</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>206</v>
+        <v>90</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4312,10 +4321,14 @@
       <c r="H4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I4" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4328,8 +4341,12 @@
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -4339,10 +4356,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -4406,7 +4423,7 @@
         <v>80</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -4438,7 +4455,7 @@
         <v>158</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -4458,6 +4475,12 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="6"/>
+      <c r="J15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4548,7 +4571,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -4581,7 +4604,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>161</v>
@@ -4613,10 +4636,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -4648,7 +4671,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="8"/>
@@ -4781,13 +4804,13 @@
         <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -4830,7 +4853,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>71</v>
@@ -4846,10 +4869,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="8"/>
@@ -4881,7 +4904,7 @@
         <v>68</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -4910,10 +4933,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -4951,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B71E50-493D-4640-A992-202C8A3B64C0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5006,7 +5029,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>164</v>
+        <v>288</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5021,10 +5044,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>89</v>
@@ -5063,16 +5086,16 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="I4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -5099,10 +5122,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -5182,7 +5205,7 @@
         <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -5284,7 +5307,7 @@
         <v>93</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5299,10 +5322,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>100</v>
@@ -5327,10 +5350,10 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -5375,10 +5398,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -5442,7 +5465,7 @@
         <v>81</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="8"/>
@@ -5458,7 +5481,7 @@
         <v>82</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="8"/>
@@ -5471,10 +5494,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="8"/>
@@ -5487,10 +5510,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
@@ -5563,7 +5586,7 @@
         <v>102</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5578,16 +5601,16 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -5606,10 +5629,10 @@
         <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -5654,10 +5677,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -5779,7 +5802,7 @@
         <v>105</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -5795,7 +5818,7 @@
         <v>107</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5811,7 +5834,7 @@
         <v>109</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -5878,7 +5901,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -5893,10 +5916,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>89</v>
@@ -5924,7 +5947,7 @@
         <v>90</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -5967,10 +5990,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -6082,7 +6105,7 @@
         <v>126</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="8"/>
@@ -6155,7 +6178,7 @@
         <v>127</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -6170,10 +6193,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>134</v>
@@ -6242,10 +6265,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>
@@ -6375,7 +6398,7 @@
         <v>137</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -6454,7 +6477,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -6469,10 +6492,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>149</v>
@@ -6541,10 +6564,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8"/>

</xml_diff>